<commit_message>
Added first version of clicking based on excel data
</commit_message>
<xml_diff>
--- a/SoftwareBot/Yritykset.xlsx
+++ b/SoftwareBot/Yritykset.xlsx
@@ -1,34 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New folder (2)\Projekti-2-Ohjelmistorobotti\SoftwareBot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB9CFE1E-E301-4AB7-8FB0-49A6634369F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7726BBBC-B63C-456A-8E24-1DA6048880B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17925" yWindow="4920" windowWidth="18390" windowHeight="13935" xr2:uid="{A81E9411-4608-4B13-9D6F-E7919D58494B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Taul1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -36,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Yritys </t>
+    <t>Name</t>
   </si>
   <si>
-    <t>Ohjelmistorobotti</t>
+    <t xml:space="preserve">                          Ostot                      </t>
   </si>
 </sst>
 </file>
@@ -95,7 +81,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -111,7 +97,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -123,7 +109,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -170,23 +156,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -222,23 +191,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -390,16 +342,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1419B93-D66F-43E5-9A8B-142B7E5C05E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
For Each loop is now working
</commit_message>
<xml_diff>
--- a/SoftwareBot/Yritykset.xlsx
+++ b/SoftwareBot/Yritykset.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB8266B-49D1-4B6D-8E08-736318E2C1AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E919401-DFC4-48A8-8FAA-398DEFB76CA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,10 @@
     <t>Name</t>
   </si>
   <si>
-    <t>RoboCamp demoyritys 1</t>
+    <t xml:space="preserve">                                         RoboCamp demoyritys 1                                     </t>
   </si>
   <si>
-    <t>Ohjelmistorobotti</t>
+    <t xml:space="preserve">                                         Ohjelmistorobotti                                     </t>
   </si>
 </sst>
 </file>
@@ -359,7 +359,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Copy file works, renaming files added.
</commit_message>
<xml_diff>
--- a/SoftwareBot/Yritykset.xlsx
+++ b/SoftwareBot/Yritykset.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E919401-DFC4-48A8-8FAA-398DEFB76CA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3DD81C-A4CB-4C0F-9BCD-DE3950911F3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t xml:space="preserve">                                         Ohjelmistorobotti                                     </t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Helmikuu</t>
+  </si>
+  <si>
+    <t>Maaliskuu</t>
   </si>
 </sst>
 </file>
@@ -356,33 +365,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged stuff from master
</commit_message>
<xml_diff>
--- a/SoftwareBot/Yritykset.xlsx
+++ b/SoftwareBot/Yritykset.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E919401-DFC4-48A8-8FAA-398DEFB76CA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3DD81C-A4CB-4C0F-9BCD-DE3950911F3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t xml:space="preserve">                                         Ohjelmistorobotti                                     </t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Helmikuu</t>
+  </si>
+  <si>
+    <t>Maaliskuu</t>
   </si>
 </sst>
 </file>
@@ -356,33 +365,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Korjaukset tehty tiedostojen siirtämiseen.
</commit_message>
<xml_diff>
--- a/SoftwareBot/Yritykset.xlsx
+++ b/SoftwareBot/Yritykset.xlsx
@@ -42,10 +42,10 @@
     <x:t>Maaliskuu</x:t>
   </x:si>
   <x:si>
+    <x:t>Ohjelmistorobotti.Maaliskuu.pdf</x:t>
+  </x:si>
+  <x:si>
     <x:t>RoboCampdemoyritys1.Helmikuu.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ohjelmistorobotti.Maaliskuu.pdf</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -94,9 +94,18 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="8">
+  <x:cellStyleXfs count="11">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -478,14 +487,19 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:sheetData>
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
     <x:row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <x:c r="A20" s="4" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <x:c r="A21" s="4" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>